<commit_message>
feat : working with image completed
</commit_message>
<xml_diff>
--- a/coffee.xlsx
+++ b/coffee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work-place\flutter apps\projects\sharp\BisleriumCafeBackend\BisleriumCafeBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956D4696-2342-4B83-AF5A-BEDB225E90E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E64F6CF-2A5E-4850-AC30-28D607EB10BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Id</t>
   </si>
@@ -40,6 +40,9 @@
     <t>Price</t>
   </si>
   <si>
+    <t>FilePath</t>
+  </si>
+  <si>
     <t>wheap cream</t>
   </si>
   <si>
@@ -50,6 +53,15 @@
   </si>
   <si>
     <t>Lazy shit</t>
+  </si>
+  <si>
+    <t>chill</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>D:\work-place\flutter apps\projects\sharp\BisleriumCafeBackend\fyp-document\fyp\coffee\coffee-image\2024-01-08\1704735419442-5ce111d5-dd7c-41f3-b432-7abff9a14dd6.jpg</t>
   </si>
 </sst>
 </file>
@@ -367,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -380,7 +392,7 @@
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,49 +402,77 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>343</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>535.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: will start working on pdf generate
</commit_message>
<xml_diff>
--- a/coffee.xlsx
+++ b/coffee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work-place\flutter apps\projects\sharp\BisleriumCafeBackend\BisleriumCafeBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E64F6CF-2A5E-4850-AC30-28D607EB10BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F70C7C-7DDC-421A-BE89-79CD0FEB0BC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Id</t>
   </si>
@@ -41,21 +41,6 @@
   </si>
   <si>
     <t>FilePath</t>
-  </si>
-  <si>
-    <t>wheap cream</t>
-  </si>
-  <si>
-    <t>laptiono</t>
-  </si>
-  <si>
-    <t>lattee</t>
-  </si>
-  <si>
-    <t>Lazy shit</t>
-  </si>
-  <si>
-    <t>chill</t>
   </si>
   <si>
     <t>water</t>
@@ -379,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,71 +393,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>535.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>